<commit_message>
Update docs to with temp issue.
</commit_message>
<xml_diff>
--- a/Modbus Codes.xlsx
+++ b/Modbus Codes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\NextCloud\Projects\Home Automation\AC Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\repos\MagIQTouch-Modbus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3142E319-96AD-4BA9-8156-02F745A48E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE37FE4-B395-47F9-BD98-9836D0BD9E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{4367DE8F-3522-4C5F-9C92-8C3D87236F94}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="120">
   <si>
     <t>Slave ID (HEX)</t>
   </si>
@@ -183,22 +183,6 @@
     <t>00 6E 00 01</t>
   </si>
   <si>
-    <t>0 9B 0 2 4 XX YY</t>
-  </si>
-  <si>
-    <t>0 9B 0 2
-Variable Entry: XX YY – Seems to be linked to number of seconds – or internal flame sensor temp?
-Observed responses:
-0 9B 0 2 4 0 24 2C F2
-0 9B 0 2 4 0 45 2C F2
-0 9B 0 2 4 0 67 2C F2
-0 9B 0 2 4 0 88 2C F2
-0 9B 0 2 4 0 AA 2C F2
-0 9B 0 2 4 0 CA 2C F2
-0 9B 0 2 4 0 EC 2C F2
-0 9B 0 2 4 1 2F 2C F2</t>
-  </si>
-  <si>
     <t>Control Panel 2</t>
   </si>
   <si>
@@ -225,17 +209,6 @@
 00 C7 00 05 0A FF D2 2C F2 30 52 64 00 80 00
 00 C7 00 05 0A FF D8 2C F2 30 52 64 00 80 00
 00 C7 00 05 0A FF DF 2C F2 30 52 64 00 80 00</t>
-  </si>
-  <si>
-    <t>Last 0 Byte occasionally is not sent – possible secondary message.
-00C7 = First register for time update.
-0005 = Registers to Write
-0A = 10 Bytes.
-XXXX = Seconds
-YYYY = Seconds Multiplier
-ZZZZ = Unknown Usage 6400 or 0000 Observed.
-Time is calculated by YYYY Dec Value x 65535 + XXXX Dec Value
-Time start 1/1/2000 02:55:00 Approx. – odd start time.</t>
   </si>
   <si>
     <t>00 CD 00 02 04 00 XX 00 A8
@@ -682,6 +655,40 @@
 +3 Recycle Mode
 x42 = Heater Fan Speed
 x90 = Zone 2 Temp Target</t>
+  </si>
+  <si>
+    <t>Control panel 2 uptime.
+00C7 = First register for time update.
+0005 = Registers to Write
+0A = 10 Bytes.
+XXXX = Seconds
+YYYY = Seconds Multiplier
+ZZZZ = Unknown Usage 6400 or 0000 Observed.
+Time is calculated by YYYY Dec Value x 65535 + XXXX Dec Value
+Time start 1/1/2000 02:55:00 Approx. – odd start time.</t>
+  </si>
+  <si>
+    <t>No Changes Observed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 9B 0 2
+</t>
+  </si>
+  <si>
+    <t>0 9B 0 2 4 XX YY
+Variable Entry: XX YY – Seems to be linked to number of seconds – or internal flame sensor temp?
+Observed responses:
+0 9B 0 2 4 0 24 2C F2
+0 9B 0 2 4 0 45 2C F2
+0 9B 0 2 4 0 67 2C F2
+0 9B 0 2 4 0 88 2C F2
+0 9B 0 2 4 0 AA 2C F2
+0 9B 0 2 4 0 CA 2C F2
+0 9B 0 2 4 0 EC 2C F2
+0 9B 0 2 4 1 2F 2C F2</t>
+  </si>
+  <si>
+    <t>Information update from CP1 - unsure of what.</t>
   </si>
 </sst>
 </file>
@@ -1160,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8075395A-3817-4F71-81A3-054D31CB2BEB}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,8 +1178,7 @@
     <col min="3" max="3" width="17.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="37.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="90.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="91.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="255.5703125" style="1" customWidth="1"/>
+    <col min="6" max="7" width="255.5703125" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1190,10 +1196,10 @@
         <v>4</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>6</v>
@@ -1315,10 +1321,10 @@
         <v>15</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="180" x14ac:dyDescent="0.25">
@@ -1382,10 +1388,10 @@
         <v>23</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="120" x14ac:dyDescent="0.25">
@@ -1408,7 +1414,7 @@
         <v>26</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1425,7 +1431,7 @@
         <v>20</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>27</v>
@@ -1468,13 +1474,15 @@
       <c r="D14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>31</v>
+      <c r="E14" s="6" t="s">
+        <v>118</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G14" s="2"/>
+        <v>117</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -1487,13 +1495,13 @@
         <v>2</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G15" s="6"/>
     </row>
@@ -1508,16 +1516,16 @@
         <v>2</v>
       </c>
       <c r="D16" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="14" t="s">
-        <v>35</v>
-      </c>
       <c r="F16" s="15" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1528,15 +1536,15 @@
         <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="165" x14ac:dyDescent="0.25">
@@ -1550,16 +1558,16 @@
         <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>39</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1573,16 +1581,16 @@
         <v>2</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1596,21 +1604,21 @@
         <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B21" s="2">
         <v>3</v>
@@ -1620,31 +1628,31 @@
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B22" s="2">
         <v>3</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B23" s="2">
         <v>3</v>
@@ -1656,16 +1664,16 @@
         <v>20</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B24" s="2">
         <v>10</v>
@@ -1677,56 +1685,56 @@
         <v>20</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B25" s="2">
         <v>3</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B26" s="2">
         <v>3</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B27" s="2">
         <v>10</v>
@@ -1738,18 +1746,18 @@
         <v>20</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B28" s="2">
         <v>3</v>
@@ -1758,21 +1766,21 @@
         <v>2</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="360" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B29" s="9">
         <v>3</v>
@@ -1781,21 +1789,21 @@
         <v>2</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="270" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B30" s="9">
         <v>3</v>
@@ -1805,12 +1813,12 @@
       <c r="E30" s="9"/>
       <c r="F30" s="10"/>
       <c r="G30" s="10" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B31" s="2">
         <v>3</v>
@@ -1819,21 +1827,21 @@
         <v>2</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B32" s="2">
         <v>10</v>
@@ -1842,19 +1850,21 @@
         <v>2</v>
       </c>
       <c r="D32" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E32" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G32" s="2"/>
+      <c r="G32" s="2" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B33" s="2">
         <v>10</v>
@@ -1863,19 +1873,21 @@
         <v>2</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G33" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B34" s="2">
         <v>10</v>
@@ -1884,19 +1896,21 @@
         <v>2</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G34" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B35" s="2">
         <v>10</v>
@@ -1905,19 +1919,21 @@
         <v>2</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G35" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B36" s="2">
         <v>10</v>
@@ -1926,19 +1942,21 @@
         <v>2</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="G36" s="2"/>
+        <v>68</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B37" s="2">
         <v>10</v>
@@ -1947,19 +1965,21 @@
         <v>2</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G37" s="2"/>
+        <v>70</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B38" s="2">
         <v>10</v>
@@ -1968,19 +1988,21 @@
         <v>2</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G38" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B39" s="2">
         <v>10</v>
@@ -1989,21 +2011,21 @@
         <v>2</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B40" s="11">
         <v>10</v>
@@ -2012,21 +2034,21 @@
         <v>2</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F40" s="12" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B41" s="16">
         <v>10</v>
@@ -2035,16 +2057,16 @@
         <v>2</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E41" s="17" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F41" s="16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="300" x14ac:dyDescent="0.25">
@@ -2055,12 +2077,12 @@
       <c r="E42" s="17"/>
       <c r="F42" s="16"/>
       <c r="G42" s="17" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B43" s="2">
         <v>3</v>
@@ -2070,16 +2092,16 @@
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B44" s="2">
         <v>3</v>
@@ -2089,16 +2111,16 @@
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B45" s="2">
         <v>10</v>
@@ -2108,7 +2130,7 @@
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>

</xml_diff>

<commit_message>
bugfix - additional zone state reporting.
</commit_message>
<xml_diff>
--- a/Modbus Codes.xlsx
+++ b/Modbus Codes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\repos\MagIQTouch-Modbus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE37FE4-B395-47F9-BD98-9836D0BD9E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031E0A5F-CBEB-4E0D-98D7-1E6D74F7EBDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{4367DE8F-3522-4C5F-9C92-8C3D87236F94}"/>
   </bookViews>
@@ -621,6 +621,60 @@
 </t>
   </si>
   <si>
+    <t>Control panel 2 uptime.
+00C7 = First register for time update.
+0005 = Registers to Write
+0A = 10 Bytes.
+XXXX = Seconds
+YYYY = Seconds Multiplier
+ZZZZ = Unknown Usage 6400 or 0000 Observed.
+Time is calculated by YYYY Dec Value x 65535 + XXXX Dec Value
+Time start 1/1/2000 02:55:00 Approx. – odd start time.</t>
+  </si>
+  <si>
+    <t>No Changes Observed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 9B 0 2
+</t>
+  </si>
+  <si>
+    <t>0 9B 0 2 4 XX YY
+Variable Entry: XX YY – Seems to be linked to number of seconds – or internal flame sensor temp?
+Observed responses:
+0 9B 0 2 4 0 24 2C F2
+0 9B 0 2 4 0 45 2C F2
+0 9B 0 2 4 0 67 2C F2
+0 9B 0 2 4 0 88 2C F2
+0 9B 0 2 4 0 AA 2C F2
+0 9B 0 2 4 0 CA 2C F2
+0 9B 0 2 4 0 EC 2C F2
+0 9B 0 2 4 1 2F 2C F2</t>
+  </si>
+  <si>
+    <t>Information update from CP1 - unsure of what.</t>
+  </si>
+  <si>
+    <t>EB 10 08 E6 00 32 64 00 00 00 EB 00 21 01 60 00 3C 00 00 FF 13 00 02 00 02 00 0F 00 32 05 36 11 E4 00 00 00 00 00 00 00 00 0C 00 00 16 00 1E 02 CD 01 74 00 00 00 00 00 00 00 00 00 00 04 04 04 04 04 04 00 04 00 00 00 58 00 58 00 00 00 00 00 00 00 02 00 00 00 00 19 16 17 0F 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 06 B4 
+(x0 = EB x1 = 10, ect)
+x11 = Aircon in automatic cleaning mode
+x12 = Aircon Mode
+Heater = 0
+Cooler +1 (Off State)
+Cooler Manual +5
+Cooler Auto +7
+External Fan +9
+Values +0x20 or +0xA0 observed, unknown signal.
+x20 = Seems to be 1 when automatic cleaning mode (1 sample)
+x40 = Heater Mode
+heater code
+0 = other modes.
++1 Heater Mode
++3 Recycle Mode
+x42 = Heater Fan Speed
+x90 = Zone 2 Temp Target</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 x14: right nibble fan speed
 left nibble, 0 when heater used.
@@ -633,62 +687,9 @@
 x89 = Zone 2 Temp Sensor, updated from 97 03 02 17 0F BF AD while off, when fan mode enabled matches z1.
 x87 = Zone 1 temp sensor - only updating when system is online
 x88 = Unsure, seemed to match temp sensor until heater enabled changed to 0x10. possible thermistor temp?
-x80 = Zone 1 Enabled/Disabled 01 = Enabled.
-x82 = Zone 2 Enabled/Disabled (Need to double check)
-	Range is from 0-3 - unsure of +2 value.</t>
-  </si>
-  <si>
-    <t>EB 10 08 E6 00 32 64 00 00 00 EB 00 21 01 60 00 3C 00 00 FF 13 00 02 00 02 00 0F 00 32 05 36 11 E4 00 00 00 00 00 00 00 00 0C 00 00 16 00 1E 02 CD 01 74 00 00 00 00 00 00 00 00 00 00 04 04 04 04 04 04 00 04 00 00 00 58 00 58 00 00 00 00 00 00 00 02 00 00 00 00 19 16 17 0F 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 06 B4 
-(x0 = EB x1 = 10, ect)
-x11 = Aircon in automatic cleaning mode (only 1 sample confirmed)
-x12 = Aircon Mode
-Heater = 0
-Cooler +1 (Off State)
-Cooler Manual +5
-Cooler Auto +7
-External Fan +9
-Values +0x20 or +0xA0 observed, unknown signal.
-x40 = Heater Mode
-heater code
-0 = other modes.
-+1 Heater Mode
-+3 Recycle Mode
-x42 = Heater Fan Speed
-x90 = Zone 2 Temp Target</t>
-  </si>
-  <si>
-    <t>Control panel 2 uptime.
-00C7 = First register for time update.
-0005 = Registers to Write
-0A = 10 Bytes.
-XXXX = Seconds
-YYYY = Seconds Multiplier
-ZZZZ = Unknown Usage 6400 or 0000 Observed.
-Time is calculated by YYYY Dec Value x 65535 + XXXX Dec Value
-Time start 1/1/2000 02:55:00 Approx. – odd start time.</t>
-  </si>
-  <si>
-    <t>No Changes Observed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 9B 0 2
-</t>
-  </si>
-  <si>
-    <t>0 9B 0 2 4 XX YY
-Variable Entry: XX YY – Seems to be linked to number of seconds – or internal flame sensor temp?
-Observed responses:
-0 9B 0 2 4 0 24 2C F2
-0 9B 0 2 4 0 45 2C F2
-0 9B 0 2 4 0 67 2C F2
-0 9B 0 2 4 0 88 2C F2
-0 9B 0 2 4 0 AA 2C F2
-0 9B 0 2 4 0 CA 2C F2
-0 9B 0 2 4 0 EC 2C F2
-0 9B 0 2 4 1 2F 2C F2</t>
-  </si>
-  <si>
-    <t>Information update from CP1 - unsure of what.</t>
+x80 = Zone State (Enabled/Disabled), LSB = Zone 1, 2nd LSB = Zone 2
+x82 = Zone 2 Enabled/Disabled (Need to double check, may just be same as x80 but value for Zone 2)
+(Ranges observed 0-3)</t>
   </si>
 </sst>
 </file>
@@ -1167,8 +1168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8075395A-3817-4F71-81A3-054D31CB2BEB}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="F40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1475,13 +1476,13 @@
         <v>20</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F14" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1567,7 +1568,7 @@
         <v>36</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1859,7 +1860,7 @@
         <v>60</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1882,7 +1883,7 @@
         <v>62</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1905,7 +1906,7 @@
         <v>64</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1928,7 +1929,7 @@
         <v>66</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1951,7 +1952,7 @@
         <v>68</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1974,7 +1975,7 @@
         <v>70</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1997,7 +1998,7 @@
         <v>72</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -2066,7 +2067,7 @@
         <v>73</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="300" x14ac:dyDescent="0.25">
@@ -2077,7 +2078,7 @@
       <c r="E42" s="17"/>
       <c r="F42" s="16"/>
       <c r="G42" s="17" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>